<commit_message>
US19 Test Cases (Mistake corrected)
Sorry the missing out the output expected in the test steps, i have added the expected input in, please review it again.
</commit_message>
<xml_diff>
--- a/SimpCity US19 Test Cases (NOT CHECKED BY THE TEAM).xlsx
+++ b/SimpCity US19 Test Cases (NOT CHECKED BY THE TEAM).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huiyi\Downloads\Year 3-Poly\Sem 3.2 DevOps\Test Cases (Not Checked)\Sprin 5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F30B24DF-3C5A-40C8-8064-F551D1096862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE3B554-D251-4AE7-8BED-CEB26693B8D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="US19 Sprint 5" sheetId="21" r:id="rId1"/>
@@ -183,64 +183,64 @@
   </si>
   <si>
     <t xml:space="preserve">
+After: Computation of final score is displayed</t>
+  </si>
+  <si>
+    <t>The users select options that are within the configuration menu that ranges from option "0" or  "3" to "5" but no the build a building selection.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+1. The user selects either option "option "0" or  "3" to "5 in the configuration menu to build a building when the message "Your Choice? is prompted.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+1. Your Choice? 3
+After: The program will process in accordance</t>
+  </si>
+  <si>
+    <t>The program will process in accordance.
+For example, the remaining buildings will be displayed since the users selects the option "3" in the configuration menu</t>
+  </si>
+  <si>
+    <t>The users select options that are not within the configuration menu but is an numeric integer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+1. The users select options that are not within the configuration menu but is a numeric integer when the message "Your Choice? is prompted.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+1. Your Choice? 7
+After: An error message will be displayed to notify and remind the users that an invalid was entered. The message "Your Choice? will be prompted again.</t>
+  </si>
+  <si>
+    <t>An error message will be displayed to notify and remind the users that an invalid was entered. The message "Your Choice? will be prompted again.</t>
+  </si>
+  <si>
+    <t>The users select options that are not within the configuration menu but is not an numeric integer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+1. The users select options that are not within the configuration menu but is not a numeric integer when the message "Your Choice? is prompted.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+1. Your Choice? a
+After: An error message will be displayed to notify and remind the users that an invalid was entered. The message "Your Choice? will be prompted again.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
 1. Your Choice? 1
 2. Confirm using SHP? [Y/N]: y
 Building confirmed
 3. Build where? a2
-4. Confirm using BCH on location a2? [Y/N]: 
+4. Confirm using BCH on location a2? [Y/N]: y
 5. Position confirmed
 6. The user see the building name appear in the grid location the user have verified. 
 After: Computation of final score is displayed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-After: Computation of final score is displayed</t>
-  </si>
-  <si>
-    <t>The users select options that are within the configuration menu that ranges from option "0" or  "3" to "5" but no the build a building selection.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-1. The user selects either option "option "0" or  "3" to "5 in the configuration menu to build a building when the message "Your Choice? is prompted.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-1. Your Choice? 3
-After: The program will process in accordance</t>
-  </si>
-  <si>
-    <t>The program will process in accordance.
-For example, the remaining buildings will be displayed since the users selects the option "3" in the configuration menu</t>
-  </si>
-  <si>
-    <t>The users select options that are not within the configuration menu but is an numeric integer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-1. The users select options that are not within the configuration menu but is a numeric integer when the message "Your Choice? is prompted.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-1. Your Choice? 7
-After: An error message will be displayed to notify and remind the users that an invalid was entered. The message "Your Choice? will be prompted again.</t>
-  </si>
-  <si>
-    <t>An error message will be displayed to notify and remind the users that an invalid was entered. The message "Your Choice? will be prompted again.</t>
-  </si>
-  <si>
-    <t>The users select options that are not within the configuration menu but is not an numeric integer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-1. The users select options that are not within the configuration menu but is not a numeric integer when the message "Your Choice? is prompted.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-1. Your Choice? a
-After: An error message will be displayed to notify and remind the users that an invalid was entered. The message "Your Choice? will be prompted again.</t>
   </si>
 </sst>
 </file>
@@ -1212,59 +1212,59 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1582,8 +1582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3650B6F3-17B5-4438-BAD0-B3F4312E77F5}">
   <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1618,24 +1618,24 @@
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="38"/>
-      <c r="B2" s="110" t="s">
+      <c r="B2" s="108" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="108"/>
+      <c r="C2" s="109"/>
       <c r="D2" s="15"/>
-      <c r="E2" s="110" t="s">
+      <c r="E2" s="108" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="108"/>
+      <c r="F2" s="109"/>
       <c r="G2" s="19"/>
-      <c r="H2" s="108" t="s">
+      <c r="H2" s="109" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="108"/>
-      <c r="J2" s="110" t="s">
+      <c r="I2" s="109"/>
+      <c r="J2" s="108" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="111"/>
+      <c r="K2" s="110"/>
       <c r="L2" s="4"/>
     </row>
     <row r="3" spans="1:12" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1748,20 +1748,20 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
-      <c r="B7" s="109" t="s">
+      <c r="B7" s="111" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="109"/>
+      <c r="C7" s="111"/>
       <c r="D7" s="11"/>
-      <c r="E7" s="109" t="s">
+      <c r="E7" s="111" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="109"/>
+      <c r="F7" s="111"/>
       <c r="G7" s="24"/>
-      <c r="H7" s="109" t="s">
+      <c r="H7" s="111" t="s">
         <v>21</v>
       </c>
-      <c r="I7" s="109"/>
+      <c r="I7" s="111"/>
       <c r="J7"/>
       <c r="L7" s="4"/>
     </row>
@@ -1892,37 +1892,37 @@
       </c>
     </row>
     <row r="14" spans="1:12" s="71" customFormat="1" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="113">
+      <c r="A14" s="115">
         <v>1</v>
       </c>
-      <c r="B14" s="124" t="s">
+      <c r="B14" s="117" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="117" t="s">
+      <c r="C14" s="119" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="119" t="s">
+      <c r="D14" s="121" t="s">
         <v>46</v>
       </c>
-      <c r="E14" s="120"/>
-      <c r="F14" s="121"/>
-      <c r="G14" s="115"/>
-      <c r="H14" s="116"/>
+      <c r="E14" s="122"/>
+      <c r="F14" s="123"/>
+      <c r="G14" s="124"/>
+      <c r="H14" s="125"/>
       <c r="I14" s="93"/>
       <c r="J14" s="93"/>
       <c r="K14" s="94"/>
     </row>
     <row r="15" spans="1:12" ht="319.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="112"/>
-      <c r="B15" s="125"/>
-      <c r="C15" s="118"/>
+      <c r="A15" s="116"/>
+      <c r="B15" s="118"/>
+      <c r="C15" s="120"/>
       <c r="D15" s="96" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="91" t="s">
         <v>47</v>
       </c>
-      <c r="E15" s="91" t="s">
-        <v>48</v>
-      </c>
-      <c r="F15" s="114" t="s">
+      <c r="F15" s="112" t="s">
         <v>40</v>
       </c>
       <c r="G15" s="97" t="s">
@@ -1940,18 +1940,18 @@
         <v>2</v>
       </c>
       <c r="B16" s="105" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="106" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="106" t="s">
+      <c r="D16" s="96" t="s">
         <v>50</v>
       </c>
-      <c r="D16" s="96" t="s">
+      <c r="E16" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="E16" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="F16" s="122"/>
+      <c r="F16" s="113"/>
       <c r="G16" s="98" t="s">
         <v>38</v>
       </c>
@@ -1967,18 +1967,18 @@
         <v>3</v>
       </c>
       <c r="B17" s="105" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="106" t="s">
         <v>53</v>
       </c>
-      <c r="C17" s="106" t="s">
+      <c r="D17" s="96" t="s">
         <v>54</v>
       </c>
-      <c r="D17" s="96" t="s">
+      <c r="E17" s="100" t="s">
         <v>55</v>
       </c>
-      <c r="E17" s="100" t="s">
-        <v>56</v>
-      </c>
-      <c r="F17" s="122"/>
+      <c r="F17" s="113"/>
       <c r="G17" s="101" t="s">
         <v>38</v>
       </c>
@@ -1994,18 +1994,18 @@
         <v>4</v>
       </c>
       <c r="B18" s="105" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="106" t="s">
         <v>57</v>
       </c>
-      <c r="C18" s="106" t="s">
+      <c r="D18" s="96" t="s">
         <v>58</v>
       </c>
-      <c r="D18" s="96" t="s">
-        <v>59</v>
-      </c>
       <c r="E18" s="100" t="s">
-        <v>56</v>
-      </c>
-      <c r="F18" s="123"/>
+        <v>55</v>
+      </c>
+      <c r="F18" s="114"/>
       <c r="G18" s="102" t="s">
         <v>38</v>
       </c>
@@ -2096,11 +2096,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="H7:I7"/>
@@ -2110,6 +2105,11 @@
     <mergeCell ref="C14:C15"/>
     <mergeCell ref="D14:F14"/>
     <mergeCell ref="G14:H14"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F15" xr:uid="{5568DE78-B01F-4F1C-B67C-1AE9B94B27C1}">

</xml_diff>